<commit_message>
Minor fixes and typos
Rouding floating points gave some issues leading to the implementation of true_round. QOL change so the script auto-detects which folder it is in and sets the base_folder accordingly. Minor typos and extended function descriptions
</commit_message>
<xml_diff>
--- a/tables/Figure_1_categorized_reasons_for_failiure.xlsx
+++ b/tables/Figure_1_categorized_reasons_for_failiure.xlsx
@@ -20,31 +20,31 @@
     <t xml:space="preserve">Number of failures</t>
   </si>
   <si>
+    <t xml:space="preserve">low E. coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not generally healthy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used disallowed probiotics or medication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no susceptible E. coli</t>
+  </si>
+  <si>
     <t xml:space="preserve">enrolled outside trial window</t>
   </si>
   <si>
-    <t xml:space="preserve">low E. coli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no susceptible E. coli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not generally healthy</t>
+    <t xml:space="preserve">unable to follow study protocol</t>
   </si>
   <si>
     <t xml:space="preserve">other</t>
   </si>
   <si>
     <t xml:space="preserve">reserve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample issues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unable to follow study protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">used disallowed probiotics or medication</t>
   </si>
   <si>
     <t xml:space="preserve">withdrew consent</t>
@@ -392,7 +392,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3">
@@ -400,7 +400,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>174</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
@@ -408,7 +408,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -416,7 +416,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>146</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -424,7 +424,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -432,7 +432,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -440,7 +440,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -448,7 +448,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -456,7 +456,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">

</xml_diff>